<commit_message>
Updated documents about AD9286 SPI interface
</commit_message>
<xml_diff>
--- a/documents/AD9286开发.xlsx
+++ b/documents/AD9286开发.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="重要管脚定义" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>管脚名称</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>数字时钟输出 - 互补</t>
+  </si>
+  <si>
+    <t>信号名称</t>
+  </si>
+  <si>
+    <t>SDIO</t>
+  </si>
+  <si>
+    <t>SPI串行时钟，用于对串行接口的读写进行同步</t>
+  </si>
+  <si>
+    <t>SPI串行数据输入输出，一个复用的信号可以作为输入或输出，取决于接收到的指令和时序的位置</t>
+  </si>
+  <si>
+    <t>SPI片选，低有效，可以控制读写循环</t>
   </si>
 </sst>
 </file>
@@ -165,9 +180,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -448,18 +469,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D14"/>
+      <selection activeCell="G1" sqref="G1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +494,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -486,8 +514,14 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -500,8 +534,14 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -514,8 +554,14 @@
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -529,7 +575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -543,7 +589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -557,7 +603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -571,7 +617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -585,7 +631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -599,7 +645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -613,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -627,7 +673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -641,7 +687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>